<commit_message>
Adding loading variables and making movement work
</commit_message>
<xml_diff>
--- a/ProjectApopalypse_Unity/Excel/Unit.xlsx
+++ b/ProjectApopalypse_Unity/Excel/Unit.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectApopalypse\ProjectApopalypse_Unity\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71C9139C-3258-4D49-B2A3-8B4DF89DE4D8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97C9B38-D863-4250-9207-8AC20C5CF8B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{3A2312A1-F630-46F4-AF7A-37D6220B2126}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>technicalName</t>
   </si>
@@ -33,19 +33,230 @@
     <t>actHealth</t>
   </si>
   <si>
-    <t>actDamage</t>
-  </si>
-  <si>
-    <t>elara</t>
+    <t>actBaseDamage</t>
+  </si>
+  <si>
+    <t>actBaseArmor</t>
+  </si>
+  <si>
+    <t>actTroopArmor</t>
+  </si>
+  <si>
+    <t>actStructureArmor</t>
+  </si>
+  <si>
+    <t>actDirectArmor</t>
+  </si>
+  <si>
+    <t>actSplashArmor</t>
+  </si>
+  <si>
+    <t>actTroopDamage</t>
+  </si>
+  <si>
+    <t>actCoreDamage</t>
+  </si>
+  <si>
+    <t>actChestDamage</t>
+  </si>
+  <si>
+    <t>actDirectDamage</t>
+  </si>
+  <si>
+    <t>actSplashDamage</t>
+  </si>
+  <si>
+    <t>actCooldown</t>
+  </si>
+  <si>
+    <t>actChargeTime</t>
+  </si>
+  <si>
+    <t>actSplashRadius</t>
+  </si>
+  <si>
+    <t>actRange</t>
+  </si>
+  <si>
+    <t>actMoveSpeed</t>
+  </si>
+  <si>
+    <t>defaultUnit</t>
+  </si>
+  <si>
+    <t>displayName</t>
+  </si>
+  <si>
+    <t>Default Unit</t>
+  </si>
+  <si>
+    <t>actHealthMax</t>
+  </si>
+  <si>
+    <t>actHealthMin</t>
+  </si>
+  <si>
+    <t>actHealthLocked</t>
+  </si>
+  <si>
+    <t>actBaseArmorMax</t>
+  </si>
+  <si>
+    <t>actBaseArmorMin</t>
+  </si>
+  <si>
+    <t>actBaseArmorLocked</t>
+  </si>
+  <si>
+    <t>actTroopArmorMax</t>
+  </si>
+  <si>
+    <t>actTroopArmorMin</t>
+  </si>
+  <si>
+    <t>actTroopArmorLocked</t>
+  </si>
+  <si>
+    <t>actStructureArmorMax</t>
+  </si>
+  <si>
+    <t>actStructureArmorMin</t>
+  </si>
+  <si>
+    <t>actStructureArmorLocked</t>
+  </si>
+  <si>
+    <t>actDirectArmorMax</t>
+  </si>
+  <si>
+    <t>actDirectArmorMin</t>
+  </si>
+  <si>
+    <t>actDirectArmorLocked</t>
+  </si>
+  <si>
+    <t>actSplashArmorMax</t>
+  </si>
+  <si>
+    <t>actSplashArmorMin</t>
+  </si>
+  <si>
+    <t>actSplashArmorLocked</t>
+  </si>
+  <si>
+    <t>actBaseDamageMax</t>
+  </si>
+  <si>
+    <t>actBaseDamageMin</t>
+  </si>
+  <si>
+    <t>actBaseDamageLocked</t>
+  </si>
+  <si>
+    <t>actTroopDamageMax</t>
+  </si>
+  <si>
+    <t>actTroopDamageMin</t>
+  </si>
+  <si>
+    <t>actTroopDamageLocked</t>
+  </si>
+  <si>
+    <t>actCoreDamageMax</t>
+  </si>
+  <si>
+    <t>actCoreDamageMin</t>
+  </si>
+  <si>
+    <t>actCoreDamageLocked</t>
+  </si>
+  <si>
+    <t>actChestDamageMax</t>
+  </si>
+  <si>
+    <t>actChestDamageMin</t>
+  </si>
+  <si>
+    <t>actChestDamageLocked</t>
+  </si>
+  <si>
+    <t>actDirectDamageMax</t>
+  </si>
+  <si>
+    <t>actDirectDamageMin</t>
+  </si>
+  <si>
+    <t>actDirectDamageLocked</t>
+  </si>
+  <si>
+    <t>actSplashDamageMax</t>
+  </si>
+  <si>
+    <t>actSplashDamageMin</t>
+  </si>
+  <si>
+    <t>actSplashDamageLocked</t>
+  </si>
+  <si>
+    <t>actCooldownMax</t>
+  </si>
+  <si>
+    <t>actCooldownMin</t>
+  </si>
+  <si>
+    <t>actCooldownLocked</t>
+  </si>
+  <si>
+    <t>actChargeTimeMax</t>
+  </si>
+  <si>
+    <t>actChargeTimeMin</t>
+  </si>
+  <si>
+    <t>actChargeTimeLocked</t>
+  </si>
+  <si>
+    <t>actSplashRadiusMax</t>
+  </si>
+  <si>
+    <t>actSplashRadiusMin</t>
+  </si>
+  <si>
+    <t>actSplashRadiusLocked</t>
+  </si>
+  <si>
+    <t>actRangeMax</t>
+  </si>
+  <si>
+    <t>actRangeMin</t>
+  </si>
+  <si>
+    <t>actRangeLocked</t>
+  </si>
+  <si>
+    <t>actMoveSpeedMax</t>
+  </si>
+  <si>
+    <t>actMoveSpeedMin</t>
+  </si>
+  <si>
+    <t>actMoveSpeedLocked</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -72,8 +283,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,42 +600,446 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66FF625-BC64-4C5F-8916-6942D597EF48}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:BR2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="7.8" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:70" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="AB1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
+    <row r="2" spans="1:70" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1">
+        <v>999</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1">
+        <v>999</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>10</v>
+      </c>
+      <c r="L2" s="1">
+        <v>999</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
+        <v>10</v>
+      </c>
+      <c r="P2" s="1">
+        <v>999</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1">
+        <v>10</v>
+      </c>
+      <c r="T2" s="1">
+        <v>999</v>
+      </c>
+      <c r="U2" s="1">
+        <v>1</v>
+      </c>
+      <c r="V2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="W2" s="1">
+        <v>10</v>
+      </c>
+      <c r="X2" s="1">
+        <v>999</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>10</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>999</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>10</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>999</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>10</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>999</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="1">
+        <v>10</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>999</v>
+      </c>
+      <c r="AO2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AP2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="1">
+        <v>10</v>
+      </c>
+      <c r="AR2" s="1">
+        <v>999</v>
+      </c>
+      <c r="AS2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AT2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AU2" s="1">
+        <v>10</v>
+      </c>
+      <c r="AV2" s="1">
+        <v>999</v>
+      </c>
+      <c r="AW2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AX2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AY2" s="1">
+        <v>10</v>
+      </c>
+      <c r="AZ2" s="1">
+        <v>999</v>
+      </c>
+      <c r="BA2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BB2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BC2" s="1">
+        <v>10</v>
+      </c>
+      <c r="BD2" s="1">
+        <v>999</v>
+      </c>
+      <c r="BE2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BF2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BG2" s="1">
+        <v>10</v>
+      </c>
+      <c r="BH2" s="1">
+        <v>999</v>
+      </c>
+      <c r="BI2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BK2" s="1">
+        <v>10</v>
+      </c>
+      <c r="BL2" s="1">
+        <v>999</v>
+      </c>
+      <c r="BM2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BN2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BO2" s="1">
+        <v>10</v>
+      </c>
+      <c r="BP2" s="1">
+        <v>999</v>
+      </c>
+      <c r="BQ2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BR2" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>